<commit_message>
Code added for Manage Requests
</commit_message>
<xml_diff>
--- a/DataSheet/Mars.xlsx
+++ b/DataSheet/Mars.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jyotimadan/Documents/Projects/CSharpProject/Mars/DataSheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jyotimadan/Documents/Projects/CSharpProject/Mars.Nunit/DataSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452DBA3E-A3F8-9441-B2A5-1C83041BBC35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B388A7B-DBF9-B845-9CA8-BD3DE1085139}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="540" windowWidth="28040" windowHeight="16280" activeTab="1" xr2:uid="{DF65A25B-7158-E041-B64A-E7FDC7345767}"/>
+    <workbookView xWindow="300" yWindow="520" windowWidth="28040" windowHeight="16280" activeTab="6" xr2:uid="{DF65A25B-7158-E041-B64A-E7FDC7345767}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
   <si>
     <t>Password</t>
   </si>
@@ -318,9 +318,6 @@
     <t>Education has been added</t>
   </si>
   <si>
-    <t>SearchSkill</t>
-  </si>
-  <si>
     <t>ChatMessage</t>
   </si>
   <si>
@@ -376,6 +373,30 @@
   </si>
   <si>
     <t>Pwd</t>
+  </si>
+  <si>
+    <t>Skill3</t>
+  </si>
+  <si>
+    <t>Skill4</t>
+  </si>
+  <si>
+    <t>SearchSkillToAccept</t>
+  </si>
+  <si>
+    <t>SearchSkillToWithdraw</t>
+  </si>
+  <si>
+    <t>SearchSkillToComplete</t>
+  </si>
+  <si>
+    <t>SearchSkillToDecline</t>
+  </si>
+  <si>
+    <t>Skill5</t>
+  </si>
+  <si>
+    <t>Skill6</t>
   </si>
 </sst>
 </file>
@@ -834,12 +855,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -851,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDD637B-99C7-7B42-BAE6-F88E174063E1}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -867,10 +888,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>48</v>
@@ -887,7 +908,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2">
         <v>123123</v>
@@ -1133,7 +1154,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1146,30 +1167,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
         <v>103</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>104</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>105</v>
-      </c>
-      <c r="D2" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1322,29 +1343,51 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABAFBA3-8E38-1348-967F-3A970261E0D5}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1363,12 +1406,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1392,18 +1435,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>